<commit_message>
Updated plan with guest lecture
</commit_message>
<xml_diff>
--- a/diverse/tidsplan-V22.xlsx
+++ b/diverse/tidsplan-V22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hakon\repositories\met4\diverse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842DC80C-2DDE-4DD0-817F-C64D4CC945FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E0B85C-1F03-49E3-997A-F804683205D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -150,12 +150,6 @@
     <t>05.04: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
   </si>
   <si>
-    <t>Gjesteforelesning?</t>
-  </si>
-  <si>
-    <t>07.04: Gjesteforelesning?</t>
-  </si>
-  <si>
     <t>19.04:  **Oversiktsforelesning: Grunnleggende statistikk/Tips til hj.eksamen** på  [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
   </si>
   <si>
@@ -163,6 +157,12 @@
   </si>
   <si>
     <t>13.01: **Introduksjon til R** på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>07.04: Gjesteforelesning med Ole-Petter Moe Hansen, Tryg forsikring</t>
+  </si>
+  <si>
+    <t>Gjesteforelesning</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +526,7 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -688,13 +688,13 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -713,10 +713,10 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oppdatert fremdriftsplan med fysisk undervisning
</commit_message>
<xml_diff>
--- a/diverse/tidsplan-V22.xlsx
+++ b/diverse/tidsplan-V22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hakon\repositories\met4\diverse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hakon/repositories/met4/diverse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E0B85C-1F03-49E3-997A-F804683205D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DC33AD-BD84-A545-86B4-4A599CF5A4EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,84 +78,9 @@
     <t>11.01: **Introduksjonsforelesning** på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
   </si>
   <si>
-    <t>18.01: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
-    <t>20.01: Oppgaveseminar på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09). Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
-    <t>25.01: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
-    <t>27.01: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
-    <t>01.02: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
-    <t>03.02: Oppgaveseminar på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09). Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
-    <t>08.02: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
-    <t>10.02: **Oversiktsforelesning: Hypotesetesting** på  [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
-    <t>15.02: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
-    <t>22.02: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
-    <t>17.02: Oppgaveseminar på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09). Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
-    <t>24.02: Oppgaveseminar på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09). Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
-    <t>01.03: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
-    <t>08.03: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
-    <t>08.03: Oppgaveseminar på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09). Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
-    <t>15.03: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
-    <t>03.03: **Oversiktsforelesning: Regresjon** på  [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
-    <t>17.03:  **Oversiktsforelesning: Logistisk, panel, kNN** på  [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
     <t>Repetisjon</t>
   </si>
   <si>
-    <t>22.03: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
-    <t>24.03: Oppgaveseminar på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09). Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
-    <t>29.03: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
-    <t>31.03:  **Oversiktsforelesning: Tidsrekker** på  [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
-    <t>05.04: Kontakttime, kursansvarlig tilgjengelig på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
-    <t>19.04:  **Oversiktsforelesning: Grunnleggende statistikk/Tips til hj.eksamen** på  [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
-    <t>21.04: **Eksamensoppgaver: Skoleeksamen** på  [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
     <t>13.01: **Introduksjon til R** på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
   </si>
   <si>
@@ -163,6 +88,81 @@
   </si>
   <si>
     <t>Gjesteforelesning</t>
+  </si>
+  <si>
+    <t>18.01: Kontakttime, kursansvarlig tilgjengelig i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>20.01: Oppgaveseminar i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09). Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>25.01: Kontakttime, kursansvarlig tilgjengelig i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>27.01: Kontakttime, kursansvarlig tilgjengelig i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>01.02: Kontakttime, kursansvarlig tilgjengelig i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>03.02: Oppgaveseminar i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09). Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>08.02: Kontakttime, kursansvarlig tilgjengelig i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>15.02: Kontakttime, kursansvarlig tilgjengelig i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>17.02: Oppgaveseminar i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09). Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>22.02: Kontakttime, kursansvarlig tilgjengelig i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>24.02: Oppgaveseminar i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09). Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>01.03: Kontakttime, kursansvarlig tilgjengelig i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>03.03: **Oversiktsforelesning: Regresjon** i Aud Max og på  [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>08.03: Kontakttime, kursansvarlig tilgjengelig i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>08.03: Oppgaveseminar i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09). Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>15.03: Kontakttime, kursansvarlig tilgjengelig i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>17.03:  **Oversiktsforelesning: Logistisk, panel, kNN** i Aud Max og på  [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>22.03: Kontakttime, kursansvarlig tilgjengelig i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>24.03: Oppgaveseminar i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09). Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>29.03: Kontakttime, kursansvarlig tilgjengelig i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>31.03:  **Oversiktsforelesning: Tidsrekker** i Aud Max og på  [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>05.04: Kontakttime, kursansvarlig tilgjengelig i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>19.04:  **Oversiktsforelesning: Grunnleggende statistikk/Tips til hj.eksamen** i Aud Max og på  [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>21.04: **Eksamensoppgaver: Skoleeksamen** i Aud Max og på  [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
+  </si>
+  <si>
+    <t>10.02: **Oversiktsforelesning: Hypotesetesting** i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
   </si>
 </sst>
 </file>
@@ -489,19 +489,19 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="83.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.5" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="83.5" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +515,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -526,10 +526,10 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -537,13 +537,13 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -551,13 +551,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -565,13 +565,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
@@ -579,13 +579,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
@@ -593,13 +593,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
@@ -607,13 +607,13 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
@@ -621,13 +621,13 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
@@ -635,13 +635,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11</v>
       </c>
@@ -649,13 +649,13 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>12</v>
       </c>
@@ -663,13 +663,13 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>13</v>
       </c>
@@ -677,27 +677,27 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>15</v>
       </c>
@@ -705,18 +705,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oppdatert eksamen og tidsplan
</commit_message>
<xml_diff>
--- a/diverse/tidsplan-V22.xlsx
+++ b/diverse/tidsplan-V22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hakon\repositories\met4\diverse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hakon/repositories/met4/diverse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE88CF9-D963-4521-9DC3-460BEB06D200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3069B3-1CE9-C846-A74D-81D1BF3AF222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -156,13 +156,13 @@
     <t>19.04:  **Oversiktsforelesning: Grunnleggende statistikk/Tips til hj.eksamen** i Aud Max og på  [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
   </si>
   <si>
-    <t>21.04: **Eksamensoppgaver: Skoleeksamen** i Aud Max og på  [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
-  </si>
-  <si>
     <t>10.02: **Oversiktsforelesning: Hypotesetesting** i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
   </si>
   <si>
     <t>10.03: Oppgaveseminar i Aud Max og på [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09). Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>21.04: Orakel med kursansvarlig i Aud Max og på  [Zoom](https://nhh.zoom.us/j/66065667678?pwd=ME1LK294VUw4SEt3eHI2V1ZuZm5MZz09).</t>
   </si>
 </sst>
 </file>
@@ -489,19 +489,19 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="83.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.5" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="83.5" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +515,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -529,7 +529,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -543,7 +543,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -557,7 +557,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -571,7 +571,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
@@ -582,10 +582,10 @@
         <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
@@ -599,7 +599,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
@@ -613,7 +613,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
@@ -627,7 +627,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
@@ -638,10 +638,10 @@
         <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11</v>
       </c>
@@ -655,7 +655,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>12</v>
       </c>
@@ -669,7 +669,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>13</v>
       </c>
@@ -683,7 +683,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>14</v>
       </c>
@@ -697,7 +697,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>15</v>
       </c>
@@ -705,7 +705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
@@ -716,7 +716,7 @@
         <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>